<commit_message>
added missing docker references. updated to ubuntu 16.04 base image.
</commit_message>
<xml_diff>
--- a/test/demo.xlsx
+++ b/test/demo.xlsx
@@ -1,20 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<s:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <s:workbookPr codeName="ThisWorkbook"/>
-  <s:bookViews>
-    <s:workbookView activeTab="0"/>
-  </s:bookViews>
-  <s:sheets>
-    <s:sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-  </s:sheets>
-  <s:definedNames/>
-  <s:calcPr calcId="124519" fullCalcOnLoad="1"/>
-</s:workbook>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\public\cmis-capture\test\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="7980"/>
+  </bookViews>
+  <sheets>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+  </sheets>
+  <calcPr calcId="0"/>
+</workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>location</t>
   </si>
@@ -28,47 +33,33 @@
     <t>test/data-barcode-skeleton/doc001/Invoice01.pdf</t>
   </si>
   <si>
-    <t xml:space="preserve">|N0001
-</t>
-  </si>
-  <si>
     <t>test/data-barcode-skeleton/doc002/Invoice02.pdf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sub Total $199.95 I
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Invoice #10
-Fun _-.-l—I
-</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <b val="1"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -84,17 +75,25 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -384,55 +383,42 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col bestFit="1" customWidth="1" max="1" min="1" width="46.5703125"/>
-    <col bestFit="1" customWidth="1" max="3" min="3" width="15.28515625"/>
+    <col min="1" max="1" width="46.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c s="1" r="A1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c s="1" r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c s="1" r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-    </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
</xml_diff>